<commit_message>
Addition of some stadistics and a better creation of the variables
</commit_message>
<xml_diff>
--- a/pocha.xlsx
+++ b/pocha.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ruiz17\pocha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92FBF562-E803-4606-9752-612EE3B31B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE1F17E-AEC8-4020-831C-49C0AF67195D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-255" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-255" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Partida 1" sheetId="1" r:id="rId1"/>
     <sheet name="Partida 2" sheetId="2" r:id="rId2"/>
     <sheet name="Partida 3" sheetId="3" r:id="rId3"/>
     <sheet name="Partida 4" sheetId="4" r:id="rId4"/>
+    <sheet name="Partida 5" sheetId="5" r:id="rId5"/>
+    <sheet name="Partida 6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="3">
   <si>
     <t>T</t>
   </si>
@@ -367,7 +369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
@@ -1708,4 +1710,672 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5798CCA-E699-44FA-AD81-02D93AC6AB0C}">
+  <dimension ref="A1:C28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>-5</v>
+      </c>
+      <c r="C2">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>-5</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>-5</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>-5</v>
+      </c>
+      <c r="B7">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-10</v>
+      </c>
+      <c r="B8">
+        <v>-5</v>
+      </c>
+      <c r="C8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>25</v>
+      </c>
+      <c r="C9">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>-5</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>-10</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>-5</v>
+      </c>
+      <c r="C12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>-5</v>
+      </c>
+      <c r="B13">
+        <v>-5</v>
+      </c>
+      <c r="C13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-5</v>
+      </c>
+      <c r="B14">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>-5</v>
+      </c>
+      <c r="B15">
+        <v>-5</v>
+      </c>
+      <c r="C15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>35</v>
+      </c>
+      <c r="B16">
+        <v>-10</v>
+      </c>
+      <c r="C16">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>30</v>
+      </c>
+      <c r="B17">
+        <v>40</v>
+      </c>
+      <c r="C17">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>-5</v>
+      </c>
+      <c r="C18">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>-10</v>
+      </c>
+      <c r="B19">
+        <v>45</v>
+      </c>
+      <c r="C19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>-5</v>
+      </c>
+      <c r="B20">
+        <v>30</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>-10</v>
+      </c>
+      <c r="B21">
+        <v>15</v>
+      </c>
+      <c r="C21">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>30</v>
+      </c>
+      <c r="B22">
+        <v>-10</v>
+      </c>
+      <c r="C22">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>-5</v>
+      </c>
+      <c r="B23">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>-5</v>
+      </c>
+      <c r="B24">
+        <v>-5</v>
+      </c>
+      <c r="C24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>-5</v>
+      </c>
+      <c r="B25">
+        <v>25</v>
+      </c>
+      <c r="C25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>-10</v>
+      </c>
+      <c r="B26">
+        <v>15</v>
+      </c>
+      <c r="C26">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>-5</v>
+      </c>
+      <c r="B27">
+        <v>20</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>10</v>
+      </c>
+      <c r="B28">
+        <v>-5</v>
+      </c>
+      <c r="C28">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E51B4F7A-CDD9-4A85-9D51-55780639B34F}">
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>-5</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>-5</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>-5</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>-5</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>-5</v>
+      </c>
+      <c r="B7">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>-5</v>
+      </c>
+      <c r="C8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>-10</v>
+      </c>
+      <c r="C9">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>30</v>
+      </c>
+      <c r="C10">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>-10</v>
+      </c>
+      <c r="C11">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>-5</v>
+      </c>
+      <c r="B13">
+        <v>-10</v>
+      </c>
+      <c r="C13">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>-5</v>
+      </c>
+      <c r="C14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <v>-5</v>
+      </c>
+      <c r="C15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>35</v>
+      </c>
+      <c r="B16">
+        <v>-5</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>-5</v>
+      </c>
+      <c r="B17">
+        <v>35</v>
+      </c>
+      <c r="C17">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>30</v>
+      </c>
+      <c r="B18">
+        <v>40</v>
+      </c>
+      <c r="C18">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>30</v>
+      </c>
+      <c r="B19">
+        <v>-5</v>
+      </c>
+      <c r="C19">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>30</v>
+      </c>
+      <c r="B20">
+        <v>-5</v>
+      </c>
+      <c r="C20">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>35</v>
+      </c>
+      <c r="C21">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>-5</v>
+      </c>
+      <c r="B22">
+        <v>30</v>
+      </c>
+      <c r="C22">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>-5</v>
+      </c>
+      <c r="C23">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>-5</v>
+      </c>
+      <c r="B24">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>-5</v>
+      </c>
+      <c r="B25">
+        <v>20</v>
+      </c>
+      <c r="C25">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>-5</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>-5</v>
+      </c>
+      <c r="B27">
+        <v>-10</v>
+      </c>
+      <c r="C27">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>20</v>
+      </c>
+      <c r="B28">
+        <v>15</v>
+      </c>
+      <c r="C28">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>20</v>
+      </c>
+      <c r="B29">
+        <v>-5</v>
+      </c>
+      <c r="C29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>15</v>
+      </c>
+      <c r="B30">
+        <v>-5</v>
+      </c>
+      <c r="C30">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Interface in now the main file and i created interfaces to have a better experience
</commit_message>
<xml_diff>
--- a/pocha.xlsx
+++ b/pocha.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ruiz17\pocha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE1F17E-AEC8-4020-831C-49C0AF67195D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AE57CA-9F07-49A0-8DFE-26ECC7EF31E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-255" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Partida 1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Partida 4" sheetId="4" r:id="rId4"/>
     <sheet name="Partida 5" sheetId="5" r:id="rId5"/>
     <sheet name="Partida 6" sheetId="6" r:id="rId6"/>
+    <sheet name="Partida 7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="3">
   <si>
     <t>T</t>
   </si>
@@ -2039,7 +2040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E51B4F7A-CDD9-4A85-9D51-55780639B34F}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
@@ -2378,4 +2379,338 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D063747-486E-48E5-A2C4-FDCEC54C844E}">
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>-5</v>
+      </c>
+      <c r="C2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>-5</v>
+      </c>
+      <c r="C3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>-5</v>
+      </c>
+      <c r="B4">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>-5</v>
+      </c>
+      <c r="C5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>-5</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>-5</v>
+      </c>
+      <c r="B7">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-10</v>
+      </c>
+      <c r="B8">
+        <v>-5</v>
+      </c>
+      <c r="C8">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>-10</v>
+      </c>
+      <c r="B9">
+        <v>-5</v>
+      </c>
+      <c r="C9">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>-5</v>
+      </c>
+      <c r="C10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>-5</v>
+      </c>
+      <c r="B11">
+        <v>35</v>
+      </c>
+      <c r="C11">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>35</v>
+      </c>
+      <c r="B12">
+        <v>-10</v>
+      </c>
+      <c r="C12">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>-10</v>
+      </c>
+      <c r="B13">
+        <v>-5</v>
+      </c>
+      <c r="C13">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-5</v>
+      </c>
+      <c r="B14">
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>-10</v>
+      </c>
+      <c r="C15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>-5</v>
+      </c>
+      <c r="B16">
+        <v>25</v>
+      </c>
+      <c r="C16">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>30</v>
+      </c>
+      <c r="B17">
+        <v>-5</v>
+      </c>
+      <c r="C17">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>25</v>
+      </c>
+      <c r="C18">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>-15</v>
+      </c>
+      <c r="B19">
+        <v>-5</v>
+      </c>
+      <c r="C19">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>25</v>
+      </c>
+      <c r="B20">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>25</v>
+      </c>
+      <c r="B21">
+        <v>-5</v>
+      </c>
+      <c r="C21">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>25</v>
+      </c>
+      <c r="C22">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>15</v>
+      </c>
+      <c r="C23">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <v>20</v>
+      </c>
+      <c r="C24">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <v>25</v>
+      </c>
+      <c r="C25">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>10</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>-5</v>
+      </c>
+      <c r="B27">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>15</v>
+      </c>
+      <c r="B28">
+        <v>-5</v>
+      </c>
+      <c r="C28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>15</v>
+      </c>
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Interface to multiplayer data
</commit_message>
<xml_diff>
--- a/pocha.xlsx
+++ b/pocha.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ruiz17\pocha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AE57CA-9F07-49A0-8DFE-26ECC7EF31E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326B5F02-E461-45BB-8849-AB983ED2F5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Partida 1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Partida 5" sheetId="5" r:id="rId5"/>
     <sheet name="Partida 6" sheetId="6" r:id="rId6"/>
     <sheet name="Partida 7" sheetId="7" r:id="rId7"/>
+    <sheet name="Partida 8" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="3">
   <si>
     <t>T</t>
   </si>
@@ -86,8 +87,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2385,7 +2387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D063747-486E-48E5-A2C4-FDCEC54C844E}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -2713,4 +2715,338 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36DCE48F-9265-4D33-8388-3FC1C481A74A}">
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>-5</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>-5</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>-5</v>
+      </c>
+      <c r="B4">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>-5</v>
+      </c>
+      <c r="C5">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>-5</v>
+      </c>
+      <c r="C6">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <v>-5</v>
+      </c>
+      <c r="C7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-5</v>
+      </c>
+      <c r="B8">
+        <v>-10</v>
+      </c>
+      <c r="C8">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>-5</v>
+      </c>
+      <c r="B9">
+        <v>-5</v>
+      </c>
+      <c r="C9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>-5</v>
+      </c>
+      <c r="B10">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>-5</v>
+      </c>
+      <c r="B11">
+        <v>-5</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>35</v>
+      </c>
+      <c r="B12">
+        <v>-5</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>-5</v>
+      </c>
+      <c r="C13">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>30</v>
+      </c>
+      <c r="B14">
+        <v>35</v>
+      </c>
+      <c r="C14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>-5</v>
+      </c>
+      <c r="B15">
+        <v>25</v>
+      </c>
+      <c r="C15">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>30</v>
+      </c>
+      <c r="B17">
+        <v>45</v>
+      </c>
+      <c r="C17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>30</v>
+      </c>
+      <c r="B18">
+        <v>-5</v>
+      </c>
+      <c r="C18">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>-5</v>
+      </c>
+      <c r="B19">
+        <v>-5</v>
+      </c>
+      <c r="C19">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>-5</v>
+      </c>
+      <c r="B20">
+        <v>-5</v>
+      </c>
+      <c r="C20">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>35</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>-5</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>15</v>
+      </c>
+      <c r="B23">
+        <v>-5</v>
+      </c>
+      <c r="C23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>-5</v>
+      </c>
+      <c r="B24">
+        <v>15</v>
+      </c>
+      <c r="C24">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>15</v>
+      </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>-5</v>
+      </c>
+      <c r="C26">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>10</v>
+      </c>
+      <c r="B27">
+        <v>15</v>
+      </c>
+      <c r="C27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>10</v>
+      </c>
+      <c r="B28">
+        <v>-5</v>
+      </c>
+      <c r="C28">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>10</v>
+      </c>
+      <c r="B29">
+        <v>-5</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Check if python3 is installed
</commit_message>
<xml_diff>
--- a/pocha.xlsx
+++ b/pocha.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ruiz17\pocha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326B5F02-E461-45BB-8849-AB983ED2F5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB183D4B-7006-4385-87DA-F18A9942D267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Partida 1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Partida 6" sheetId="6" r:id="rId6"/>
     <sheet name="Partida 7" sheetId="7" r:id="rId7"/>
     <sheet name="Partida 8" sheetId="8" r:id="rId8"/>
+    <sheet name="Partida 9" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="3">
   <si>
     <t>T</t>
   </si>
@@ -87,9 +88,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2721,8 +2721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36DCE48F-9265-4D33-8388-3FC1C481A74A}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2959,7 +2959,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22">
         <v>-5</v>
       </c>
       <c r="B22">
@@ -3043,6 +3043,296 @@
         <v>-5</v>
       </c>
       <c r="C29">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83EE7463-64F9-443E-A0D4-78C6C8B2201E}">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>-5</v>
+      </c>
+      <c r="C2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>-5</v>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>-5</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>-5</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>-5</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <v>-5</v>
+      </c>
+      <c r="C7">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-5</v>
+      </c>
+      <c r="B8">
+        <v>-5</v>
+      </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>-5</v>
+      </c>
+      <c r="C9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <v>-10</v>
+      </c>
+      <c r="C10">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>-5</v>
+      </c>
+      <c r="B11">
+        <v>40</v>
+      </c>
+      <c r="C11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>-10</v>
+      </c>
+      <c r="C12">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>35</v>
+      </c>
+      <c r="B13">
+        <v>-10</v>
+      </c>
+      <c r="C13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>35</v>
+      </c>
+      <c r="B14">
+        <v>40</v>
+      </c>
+      <c r="C14">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>-5</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>-5</v>
+      </c>
+      <c r="C17">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>-5</v>
+      </c>
+      <c r="C18">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>-15</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <v>-10</v>
+      </c>
+      <c r="C20">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>-5</v>
+      </c>
+      <c r="B21">
+        <v>15</v>
+      </c>
+      <c r="C21">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>-5</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>-5</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>10</v>
+      </c>
+      <c r="B24">
+        <v>-5</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>-5</v>
+      </c>
+      <c r="B25">
+        <v>15</v>
+      </c>
+      <c r="C25">
         <v>10</v>
       </c>
     </row>

</xml_diff>